<commit_message>
End of regional sort
</commit_message>
<xml_diff>
--- a/dataset/French_Election/Election_gathering.xlsx
+++ b/dataset/French_Election/Election_gathering.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\GitHub\com-480-project-datart\dataset\French_Election\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84E1638-1684-4B8A-AF2A-0D8412BF5FF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegionT1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="80">
   <si>
     <t>Region Code</t>
   </si>
@@ -40,6 +46,75 @@
     <t>SecondScore</t>
   </si>
   <si>
+    <t>Surname27</t>
+  </si>
+  <si>
+    <t>Name27</t>
+  </si>
+  <si>
+    <t>Parti27</t>
+  </si>
+  <si>
+    <t>Year0</t>
+  </si>
+  <si>
+    <t>FirstScore0</t>
+  </si>
+  <si>
+    <t>Surname0</t>
+  </si>
+  <si>
+    <t>Name0</t>
+  </si>
+  <si>
+    <t>Parti0</t>
+  </si>
+  <si>
+    <t>Second Score0</t>
+  </si>
+  <si>
+    <t>Surname20</t>
+  </si>
+  <si>
+    <t>Name20</t>
+  </si>
+  <si>
+    <t>Parti20</t>
+  </si>
+  <si>
+    <t>Year1</t>
+  </si>
+  <si>
+    <t>FirstScore1</t>
+  </si>
+  <si>
+    <t>Surname1</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Parti1</t>
+  </si>
+  <si>
+    <t>Second Score1</t>
+  </si>
+  <si>
+    <t>Surname21</t>
+  </si>
+  <si>
+    <t>Name21</t>
+  </si>
+  <si>
+    <t>Parti21</t>
+  </si>
+  <si>
+    <t>Year2</t>
+  </si>
+  <si>
+    <t>FirstScore2</t>
+  </si>
+  <si>
     <t>Surname2</t>
   </si>
   <si>
@@ -49,28 +124,16 @@
     <t>Parti2</t>
   </si>
   <si>
-    <t>FirstScore0</t>
-  </si>
-  <si>
-    <t>Surname0</t>
-  </si>
-  <si>
-    <t>Name0</t>
-  </si>
-  <si>
-    <t>Parti0</t>
-  </si>
-  <si>
-    <t>Second Score0</t>
-  </si>
-  <si>
-    <t>Surname20</t>
-  </si>
-  <si>
-    <t>Name20</t>
-  </si>
-  <si>
-    <t>Parti20</t>
+    <t>Second Score2</t>
+  </si>
+  <si>
+    <t>Surname22</t>
+  </si>
+  <si>
+    <t>Name22</t>
+  </si>
+  <si>
+    <t>Parti22</t>
   </si>
   <si>
     <t>Grand Est</t>
@@ -127,9 +190,6 @@
     <t>Mayotte</t>
   </si>
   <si>
-    <t>2017</t>
-  </si>
-  <si>
     <t>LE PEN</t>
   </si>
   <si>
@@ -161,13 +221,52 @@
   </si>
   <si>
     <t>Nicolas</t>
+  </si>
+  <si>
+    <t>ROYAL</t>
+  </si>
+  <si>
+    <t>Ségolène</t>
+  </si>
+  <si>
+    <t>CHIRAC</t>
+  </si>
+  <si>
+    <t>JOSPIN</t>
+  </si>
+  <si>
+    <t>JEAN-MARIE</t>
+  </si>
+  <si>
+    <t>JACQUES</t>
+  </si>
+  <si>
+    <t>LIONEL</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>LREM</t>
+  </si>
+  <si>
+    <t>LFI</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>UMP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,22 +318,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -276,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,9 +416,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,6 +468,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,14 +661,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AL19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,851 +728,2150 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2017</v>
       </c>
       <c r="D2">
         <v>27.78</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
       </c>
       <c r="H2">
         <v>20.72</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
       </c>
       <c r="L2">
-        <v>28.60384713553147</v>
-      </c>
-      <c r="M2" t="s">
-        <v>46</v>
+        <v>2012</v>
+      </c>
+      <c r="M2">
+        <v>28.603847135531471</v>
       </c>
       <c r="N2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2">
-        <v>23.2728496183029</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+      <c r="O2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2">
+        <v>23.272849618302899</v>
       </c>
       <c r="R2" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="S2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U2">
+        <v>2007</v>
+      </c>
+      <c r="V2">
+        <v>32.485301998120121</v>
+      </c>
+      <c r="W2" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z2">
+        <v>20.7535177233867</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD2">
+        <v>2002</v>
+      </c>
+      <c r="AE2">
+        <v>21.91911703365113</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI2">
+        <v>18.99858809752044</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2017</v>
       </c>
       <c r="D3">
         <v>25.12</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
       </c>
       <c r="H3">
         <v>20.75</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
+        <v>76</v>
       </c>
       <c r="L3">
-        <v>33.22168332129264</v>
-      </c>
-      <c r="M3" t="s">
-        <v>47</v>
+        <v>2012</v>
+      </c>
+      <c r="M3">
+        <v>33.221683321292637</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3">
-        <v>24.18639117042781</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3">
+        <v>24.186391170427811</v>
       </c>
       <c r="R3" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U3">
+        <v>2007</v>
+      </c>
+      <c r="V3">
+        <v>30.044674989773039</v>
+      </c>
+      <c r="W3" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z3">
+        <v>27.700629670096369</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD3">
+        <v>2002</v>
+      </c>
+      <c r="AE3">
+        <v>22.80661565589773</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI3">
+        <v>17.52652874866175</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2017</v>
       </c>
       <c r="D4">
         <v>24.5</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
       </c>
       <c r="H4">
         <v>20.72</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
       </c>
       <c r="L4">
-        <v>27.4029851028094</v>
-      </c>
-      <c r="M4" t="s">
-        <v>46</v>
+        <v>2012</v>
+      </c>
+      <c r="M4">
+        <v>27.402985102809399</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4">
-        <v>26.47841328256512</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+      <c r="O4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q4">
+        <v>26.478413282565121</v>
       </c>
       <c r="R4" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="S4" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" t="s">
+        <v>78</v>
+      </c>
+      <c r="U4">
+        <v>2007</v>
+      </c>
+      <c r="V4">
+        <v>31.75318511256739</v>
+      </c>
+      <c r="W4" t="s">
+        <v>64</v>
+      </c>
+      <c r="X4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z4">
+        <v>24.115012872221449</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD4">
+        <v>2002</v>
+      </c>
+      <c r="AE4">
+        <v>18.67253104778602</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI4">
+        <v>17.978998042129142</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2017</v>
       </c>
       <c r="D5">
         <v>25.09</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
       </c>
       <c r="H5">
         <v>21.89</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
       </c>
       <c r="L5">
-        <v>27.11595066543872</v>
-      </c>
-      <c r="M5" t="s">
-        <v>47</v>
+        <v>2012</v>
+      </c>
+      <c r="M5">
+        <v>27.115950665438721</v>
       </c>
       <c r="N5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5">
-        <v>26.64544535793212</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="O5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5">
+        <v>26.645445357932122</v>
       </c>
       <c r="R5" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S5" t="s">
+        <v>66</v>
+      </c>
+      <c r="T5" t="s">
+        <v>79</v>
+      </c>
+      <c r="U5">
+        <v>2007</v>
+      </c>
+      <c r="V5">
+        <v>30.698054763372902</v>
+      </c>
+      <c r="W5" t="s">
+        <v>64</v>
+      </c>
+      <c r="X5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z5">
+        <v>24.46569822336982</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD5">
+        <v>2002</v>
+      </c>
+      <c r="AE5">
+        <v>18.97515219128595</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI5">
+        <v>18.4743200114393</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2017</v>
       </c>
       <c r="D6">
         <v>29.05</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
       </c>
       <c r="H6">
         <v>19.28</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="K6" t="s">
+        <v>76</v>
       </c>
       <c r="L6">
+        <v>2012</v>
+      </c>
+      <c r="M6">
         <v>31.74</v>
       </c>
-      <c r="M6" t="s">
-        <v>47</v>
-      </c>
       <c r="N6" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6">
+        <v>65</v>
+      </c>
+      <c r="O6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q6">
         <v>25.66</v>
       </c>
-      <c r="Q6" t="s">
-        <v>46</v>
-      </c>
       <c r="R6" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U6">
+        <v>2007</v>
+      </c>
+      <c r="V6">
+        <v>28.14</v>
+      </c>
+      <c r="W6" t="s">
+        <v>67</v>
+      </c>
+      <c r="X6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z6">
+        <v>27.81</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD6">
+        <v>2002</v>
+      </c>
+      <c r="AE6">
+        <v>21.6</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI6">
+        <v>18.07</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2017</v>
       </c>
       <c r="D7">
         <v>23.08</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
       </c>
       <c r="H7">
         <v>22.68</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="K7" t="s">
+        <v>75</v>
       </c>
       <c r="L7">
+        <v>2012</v>
+      </c>
+      <c r="M7">
         <v>28.53</v>
       </c>
-      <c r="M7" t="s">
-        <v>46</v>
-      </c>
       <c r="N7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7">
+        <v>64</v>
+      </c>
+      <c r="O7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7">
         <v>24.76</v>
       </c>
-      <c r="Q7" t="s">
-        <v>47</v>
-      </c>
       <c r="R7" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="S7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" t="s">
+        <v>78</v>
+      </c>
+      <c r="U7">
+        <v>2007</v>
+      </c>
+      <c r="V7">
+        <v>32.74</v>
+      </c>
+      <c r="W7" t="s">
+        <v>64</v>
+      </c>
+      <c r="X7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z7">
+        <v>21.27</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD7">
+        <v>2002</v>
+      </c>
+      <c r="AE7">
+        <v>21.12</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI7">
+        <v>19.97</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2017</v>
       </c>
       <c r="D8">
         <v>28.63</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
       </c>
       <c r="H8">
         <v>22.19</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>63</v>
+      </c>
+      <c r="K8" t="s">
+        <v>77</v>
       </c>
       <c r="L8">
+        <v>2012</v>
+      </c>
+      <c r="M8">
         <v>26.64</v>
       </c>
-      <c r="M8" t="s">
-        <v>46</v>
-      </c>
       <c r="N8" t="s">
-        <v>48</v>
-      </c>
-      <c r="P8">
+        <v>64</v>
+      </c>
+      <c r="O8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8">
         <v>25.89</v>
       </c>
-      <c r="Q8" t="s">
-        <v>47</v>
-      </c>
       <c r="R8" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="S8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T8" t="s">
+        <v>78</v>
+      </c>
+      <c r="U8">
+        <v>2007</v>
+      </c>
+      <c r="V8">
+        <v>30.93</v>
+      </c>
+      <c r="W8" t="s">
+        <v>64</v>
+      </c>
+      <c r="X8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z8">
+        <v>24.07</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD8">
+        <v>2002</v>
+      </c>
+      <c r="AE8">
+        <v>19.98</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI8">
+        <v>17.7</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2017</v>
       </c>
       <c r="D9">
         <v>22.98</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
       </c>
       <c r="H9">
         <v>22.32</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>75</v>
       </c>
       <c r="L9">
+        <v>2012</v>
+      </c>
+      <c r="M9">
         <v>29.27351767345435</v>
       </c>
-      <c r="M9" t="s">
-        <v>47</v>
-      </c>
       <c r="N9" t="s">
-        <v>45</v>
-      </c>
-      <c r="P9">
-        <v>23.79671037209996</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="O9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9">
+        <v>23.796710372099959</v>
       </c>
       <c r="R9" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S9" t="s">
+        <v>66</v>
+      </c>
+      <c r="T9" t="s">
+        <v>79</v>
+      </c>
+      <c r="U9">
+        <v>2007</v>
+      </c>
+      <c r="V9">
+        <v>28.54450136808547</v>
+      </c>
+      <c r="W9" t="s">
+        <v>67</v>
+      </c>
+      <c r="X9" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z9">
+        <v>28.257153182644512</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD9">
+        <v>2002</v>
+      </c>
+      <c r="AE9">
+        <v>18.556509805349052</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI9">
+        <v>17.991098086018791</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2017</v>
       </c>
       <c r="D10">
         <v>31.04</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>74</v>
       </c>
       <c r="H10">
         <v>19.59</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>76</v>
       </c>
       <c r="L10">
+        <v>2012</v>
+      </c>
+      <c r="M10">
         <v>27.90330912183153</v>
       </c>
-      <c r="M10" t="s">
-        <v>47</v>
-      </c>
       <c r="N10" t="s">
-        <v>45</v>
-      </c>
-      <c r="P10">
-        <v>24.09298240056918</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="O10" t="s">
+        <v>63</v>
+      </c>
+      <c r="P10" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q10">
+        <v>24.092982400569181</v>
       </c>
       <c r="R10" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T10" t="s">
+        <v>79</v>
+      </c>
+      <c r="U10">
+        <v>2007</v>
+      </c>
+      <c r="V10">
+        <v>28.676020828790111</v>
+      </c>
+      <c r="W10" t="s">
+        <v>64</v>
+      </c>
+      <c r="X10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z10">
+        <v>24.376463065302431</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD10">
+        <v>2002</v>
+      </c>
+      <c r="AE10">
+        <v>19.432499451811211</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI10">
+        <v>17.59315860388477</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
+        <v>47</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2017</v>
       </c>
       <c r="D11">
         <v>23.93</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
       </c>
       <c r="H11">
         <v>22.36</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
       </c>
       <c r="L11">
-        <v>27.71135904260746</v>
-      </c>
-      <c r="M11" t="s">
-        <v>47</v>
+        <v>2012</v>
+      </c>
+      <c r="M11">
+        <v>27.711359042607459</v>
       </c>
       <c r="N11" t="s">
-        <v>45</v>
-      </c>
-      <c r="P11">
+        <v>65</v>
+      </c>
+      <c r="O11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P11" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q11">
         <v>27.02037629938609</v>
       </c>
-      <c r="Q11" t="s">
-        <v>46</v>
-      </c>
       <c r="R11" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S11" t="s">
+        <v>66</v>
+      </c>
+      <c r="T11" t="s">
+        <v>79</v>
+      </c>
+      <c r="U11">
+        <v>2007</v>
+      </c>
+      <c r="V11">
+        <v>30.055837819316011</v>
+      </c>
+      <c r="W11" t="s">
+        <v>64</v>
+      </c>
+      <c r="X11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z11">
+        <v>23.75991621526811</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD11">
+        <v>2002</v>
+      </c>
+      <c r="AE11">
+        <v>20.62745264434762</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI11">
+        <v>16.110874344115551</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2017</v>
       </c>
       <c r="D12">
         <v>26.27</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
       </c>
       <c r="H12">
         <v>23.56</v>
       </c>
       <c r="I12" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>45</v>
+        <v>63</v>
+      </c>
+      <c r="K12" t="s">
+        <v>77</v>
       </c>
       <c r="L12">
+        <v>2012</v>
+      </c>
+      <c r="M12">
         <v>31.9</v>
       </c>
-      <c r="M12" t="s">
-        <v>47</v>
-      </c>
       <c r="N12" t="s">
-        <v>45</v>
-      </c>
-      <c r="P12">
+        <v>65</v>
+      </c>
+      <c r="O12" t="s">
+        <v>63</v>
+      </c>
+      <c r="P12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q12">
         <v>22.94</v>
       </c>
-      <c r="Q12" t="s">
-        <v>46</v>
-      </c>
       <c r="R12" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S12" t="s">
+        <v>66</v>
+      </c>
+      <c r="T12" t="s">
+        <v>79</v>
+      </c>
+      <c r="U12">
+        <v>2007</v>
+      </c>
+      <c r="V12">
+        <v>31.11</v>
+      </c>
+      <c r="W12" t="s">
+        <v>67</v>
+      </c>
+      <c r="X12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z12">
+        <v>26.29</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD12">
+        <v>2002</v>
+      </c>
+      <c r="AE12">
+        <v>19.53</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI12">
+        <v>17.12</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
+        <v>49</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2017</v>
       </c>
       <c r="D13">
         <v>28.16</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
       </c>
       <c r="H13">
         <v>22.38</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="J13" t="s">
-        <v>45</v>
+        <v>63</v>
+      </c>
+      <c r="K13" t="s">
+        <v>77</v>
       </c>
       <c r="L13">
+        <v>2012</v>
+      </c>
+      <c r="M13">
         <v>28.53</v>
       </c>
-      <c r="M13" t="s">
-        <v>47</v>
-      </c>
       <c r="N13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13">
+        <v>65</v>
+      </c>
+      <c r="O13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q13">
         <v>23.62</v>
       </c>
-      <c r="Q13" t="s">
-        <v>46</v>
-      </c>
       <c r="R13" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S13" t="s">
+        <v>66</v>
+      </c>
+      <c r="T13" t="s">
+        <v>79</v>
+      </c>
+      <c r="U13">
+        <v>2007</v>
+      </c>
+      <c r="V13">
+        <v>27.92</v>
+      </c>
+      <c r="W13" t="s">
+        <v>64</v>
+      </c>
+      <c r="X13" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z13">
+        <v>25.02</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD13">
+        <v>2002</v>
+      </c>
+      <c r="AE13">
+        <v>19.04</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI13">
+        <v>17.29</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2017</v>
       </c>
       <c r="D14">
         <v>27.88</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>74</v>
       </c>
       <c r="H14">
         <v>25.56</v>
       </c>
       <c r="I14" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>63</v>
+      </c>
+      <c r="K14" t="s">
+        <v>77</v>
       </c>
       <c r="L14">
+        <v>2012</v>
+      </c>
+      <c r="M14">
         <v>28.31</v>
       </c>
-      <c r="M14" t="s">
-        <v>46</v>
-      </c>
       <c r="N14" t="s">
-        <v>48</v>
-      </c>
-      <c r="P14">
+        <v>64</v>
+      </c>
+      <c r="O14" t="s">
+        <v>66</v>
+      </c>
+      <c r="P14" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q14">
         <v>27.54</v>
       </c>
-      <c r="Q14" t="s">
-        <v>47</v>
-      </c>
       <c r="R14" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="S14" t="s">
+        <v>63</v>
+      </c>
+      <c r="T14" t="s">
+        <v>78</v>
+      </c>
+      <c r="U14">
+        <v>2007</v>
+      </c>
+      <c r="V14">
+        <v>30.84</v>
+      </c>
+      <c r="W14" t="s">
+        <v>64</v>
+      </c>
+      <c r="X14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z14">
+        <v>22.99</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD14">
+        <v>2002</v>
+      </c>
+      <c r="AE14">
+        <v>22.37</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI14">
+        <v>14.74</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
+        <v>51</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2017</v>
       </c>
       <c r="D15">
         <v>30.23</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
       </c>
       <c r="H15">
         <v>24.13</v>
       </c>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="K15" t="s">
+        <v>76</v>
       </c>
       <c r="L15">
+        <v>2012</v>
+      </c>
+      <c r="M15">
         <v>27.86</v>
       </c>
-      <c r="M15" t="s">
-        <v>47</v>
-      </c>
       <c r="N15" t="s">
-        <v>45</v>
-      </c>
-      <c r="P15">
+        <v>65</v>
+      </c>
+      <c r="O15" t="s">
+        <v>63</v>
+      </c>
+      <c r="P15" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q15">
         <v>25.92</v>
       </c>
-      <c r="Q15" t="s">
-        <v>46</v>
-      </c>
       <c r="R15" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S15" t="s">
+        <v>66</v>
+      </c>
+      <c r="T15" t="s">
+        <v>79</v>
+      </c>
+      <c r="U15">
+        <v>2007</v>
+      </c>
+      <c r="V15">
+        <v>29.38</v>
+      </c>
+      <c r="W15" t="s">
+        <v>64</v>
+      </c>
+      <c r="X15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z15">
+        <v>24.42</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD15">
+        <v>2002</v>
+      </c>
+      <c r="AE15">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI15">
+        <v>17.27</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
+        <v>52</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2017</v>
       </c>
       <c r="D16">
         <v>27.37</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="G16" t="s">
+        <v>76</v>
       </c>
       <c r="H16">
         <v>25.53</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="K16" t="s">
+        <v>75</v>
       </c>
       <c r="L16">
+        <v>2012</v>
+      </c>
+      <c r="M16">
         <v>28.63</v>
       </c>
-      <c r="M16" t="s">
-        <v>46</v>
-      </c>
       <c r="N16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P16">
+        <v>64</v>
+      </c>
+      <c r="O16" t="s">
+        <v>66</v>
+      </c>
+      <c r="P16" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q16">
         <v>28.4</v>
       </c>
-      <c r="Q16" t="s">
-        <v>47</v>
-      </c>
       <c r="R16" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="S16" t="s">
+        <v>63</v>
+      </c>
+      <c r="T16" t="s">
+        <v>78</v>
+      </c>
+      <c r="U16">
+        <v>2007</v>
+      </c>
+      <c r="V16">
+        <v>29.48</v>
+      </c>
+      <c r="W16" t="s">
+        <v>64</v>
+      </c>
+      <c r="X16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z16">
+        <v>25.56</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD16">
+        <v>2002</v>
+      </c>
+      <c r="AE16">
+        <v>21.68</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI16">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
+        <v>53</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2017</v>
       </c>
       <c r="D17">
         <v>24.71</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
+        <v>76</v>
       </c>
       <c r="H17">
         <v>24.3</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="J17" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="K17" t="s">
+        <v>74</v>
       </c>
       <c r="L17">
+        <v>2012</v>
+      </c>
+      <c r="M17">
         <v>26.59</v>
       </c>
-      <c r="M17" t="s">
-        <v>47</v>
-      </c>
       <c r="N17" t="s">
-        <v>45</v>
-      </c>
-      <c r="P17">
+        <v>65</v>
+      </c>
+      <c r="O17" t="s">
+        <v>63</v>
+      </c>
+      <c r="P17" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q17">
         <v>25.09</v>
       </c>
-      <c r="Q17" t="s">
-        <v>46</v>
-      </c>
       <c r="R17" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T17" t="s">
+        <v>79</v>
+      </c>
+      <c r="U17">
+        <v>2007</v>
+      </c>
+      <c r="V17">
+        <v>30.27</v>
+      </c>
+      <c r="W17" t="s">
+        <v>64</v>
+      </c>
+      <c r="X17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z17">
+        <v>23.02</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD17">
+        <v>2002</v>
+      </c>
+      <c r="AE17">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI17">
+        <v>18.22</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
+        <v>54</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2017</v>
       </c>
       <c r="D18">
         <v>24.53</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
       </c>
       <c r="H18">
         <v>23.46</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="J18" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="K18" t="s">
+        <v>74</v>
       </c>
       <c r="L18">
+        <v>2012</v>
+      </c>
+      <c r="M18">
         <v>31.17</v>
       </c>
-      <c r="M18" t="s">
-        <v>47</v>
-      </c>
       <c r="N18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P18">
+        <v>65</v>
+      </c>
+      <c r="O18" t="s">
+        <v>63</v>
+      </c>
+      <c r="P18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q18">
         <v>25.61</v>
       </c>
-      <c r="Q18" t="s">
-        <v>46</v>
-      </c>
       <c r="R18" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="S18" t="s">
+        <v>66</v>
+      </c>
+      <c r="T18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U18">
+        <v>2007</v>
+      </c>
+      <c r="V18">
+        <v>29.87</v>
+      </c>
+      <c r="W18" t="s">
+        <v>67</v>
+      </c>
+      <c r="X18" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z18">
+        <v>28.22</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD18">
+        <v>2002</v>
+      </c>
+      <c r="AE18">
+        <v>20.9</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI18">
+        <v>17.170000000000002</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
+        <v>55</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2017</v>
       </c>
       <c r="D19">
-        <v>32.62</v>
+        <v>32.619999999999997</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
       </c>
       <c r="H19">
         <v>27.19</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="J19" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="K19" t="s">
+        <v>74</v>
       </c>
       <c r="L19">
+        <v>2012</v>
+      </c>
+      <c r="M19">
         <v>31.06</v>
       </c>
-      <c r="M19" t="s">
-        <v>46</v>
-      </c>
       <c r="N19" t="s">
-        <v>48</v>
-      </c>
-      <c r="P19">
+        <v>64</v>
+      </c>
+      <c r="O19" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q19">
         <v>23.87</v>
       </c>
-      <c r="Q19" t="s">
-        <v>38</v>
-      </c>
       <c r="R19" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="S19" t="s">
+        <v>60</v>
+      </c>
+      <c r="T19" t="s">
+        <v>74</v>
+      </c>
+      <c r="U19">
+        <v>2007</v>
+      </c>
+      <c r="V19">
+        <v>37.01</v>
+      </c>
+      <c r="W19" t="s">
+        <v>64</v>
+      </c>
+      <c r="X19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z19">
+        <v>21.21</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD19">
+        <v>2002</v>
+      </c>
+      <c r="AE19">
+        <v>23.35</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI19">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>